<commit_message>
Updated gitignore. Updated Tag friendlyness file
</commit_message>
<xml_diff>
--- a/topic-files/Tag_Friendliness_8_Topics_and_16_Topics.xlsx
+++ b/topic-files/Tag_Friendliness_8_Topics_and_16_Topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_410_Text_Info_Systems\Project\CourseProject\topic-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creon/Desktop/UIUC/CS410/Team Project/CourseProject/topic-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{917FC1A3-5297-44F4-AE28-CE761FC8B9F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7613FE00-5F6C-E649-B325-817718764F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31780" yWindow="1180" windowWidth="18690" windowHeight="18410" xr2:uid="{C0B249B2-4F70-4EBF-AAE4-C111E07652C1}"/>
+    <workbookView xWindow="10140" yWindow="1460" windowWidth="33560" windowHeight="22640" xr2:uid="{C0B249B2-4F70-4EBF-AAE4-C111E07652C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="105">
   <si>
     <t>User-Friendly?</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Gauge user-friendliness of the top tags in the 8-topic and 16-topic models for CS 410 course projects.</t>
+  </si>
+  <si>
+    <t>Should Keep?</t>
   </si>
 </sst>
 </file>
@@ -431,7 +434,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -498,26 +507,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C961D82F-9873-4272-B1DE-C98A5689777E}" name="Table_8_Topics" displayName="Table_8_Topics" ref="A5:D49" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A5:D49" xr:uid="{C961D82F-9873-4272-B1DE-C98A5689777E}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D282E914-8222-4D84-884B-9CF7507FD194}" name="Tag" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C961D82F-9873-4272-B1DE-C98A5689777E}" name="Table_8_Topics" displayName="Table_8_Topics" ref="A5:E49" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A5:E49" xr:uid="{C961D82F-9873-4272-B1DE-C98A5689777E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D282E914-8222-4D84-884B-9CF7507FD194}" name="Tag" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{D1A6DB4D-13DB-48D7-9E2B-C9FB047881F9}" name="Kurt"/>
     <tableColumn id="3" xr3:uid="{C7736CBA-5385-41C8-8441-2C8472818DBF}" name="Creon"/>
     <tableColumn id="4" xr3:uid="{BAFD5142-42F3-48E9-BF35-4EB4D5FD81CC}" name="Suhas"/>
+    <tableColumn id="5" xr3:uid="{113810B2-765C-F54B-A7C3-390459E3EE38}" name="Should Keep?" dataDxfId="1">
+      <calculatedColumnFormula>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}" name="Table_16_Topics" displayName="Table_16_Topics" ref="G5:J93" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="G5:J93" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{891C3C5A-718E-41CB-BECD-51A095C7EA48}" name="Tag" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}" name="Table_16_Topics" displayName="Table_16_Topics" ref="G5:K93" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="G5:K93" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{891C3C5A-718E-41CB-BECD-51A095C7EA48}" name="Tag" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{342D09C5-EE2F-4797-AC7E-8C507A5D6470}" name="Kurt"/>
     <tableColumn id="3" xr3:uid="{1706DFBA-C6B1-4DC0-B09A-1674717EDFE0}" name="Creon"/>
     <tableColumn id="4" xr3:uid="{B49B5B10-9CB0-4EB0-AB00-0C83FC81E11F}" name="Suhas"/>
+    <tableColumn id="5" xr3:uid="{CBEE1EE4-5DE5-6942-AC94-BA3C3CDC6AA5}" name="Should Keep?" dataDxfId="0">
+      <calculatedColumnFormula>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -820,29 +835,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6BCABA-D507-48B2-ACA1-86EC87461762}">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -860,7 +877,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -873,6 +890,9 @@
       <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E5" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>50</v>
       </c>
@@ -885,802 +905,1561 @@
       <c r="J5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>48</v>
       </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G7" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>48</v>
       </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>48</v>
       </c>
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G9" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>48</v>
       </c>
+      <c r="C10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G10" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="E11" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G11" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H11" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>48</v>
       </c>
+      <c r="C12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G12" s="2" t="s">
         <v>57</v>
       </c>
       <c r="H12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E13" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G13" s="2" t="s">
         <v>58</v>
       </c>
       <c r="H13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="E14" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G14" s="2" t="s">
         <v>59</v>
       </c>
       <c r="H14" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>48</v>
       </c>
+      <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="H15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
       </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G16" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H16" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="E17" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G17" s="2" t="s">
         <v>61</v>
       </c>
       <c r="H17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>48</v>
       </c>
+      <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H18" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="E19" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G19" s="2" t="s">
         <v>62</v>
       </c>
       <c r="H19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="E20" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="H20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E21" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G21" s="2" t="s">
         <v>63</v>
       </c>
       <c r="H21" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="E22" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H22" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
       </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K23" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E24" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G24" s="2" t="s">
         <v>64</v>
       </c>
       <c r="H24" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
       </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G25" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K25" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>48</v>
       </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G26" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K26" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
+      <c r="C27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="H27" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="E28" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G28" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K28" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>48</v>
       </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G29" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>48</v>
       </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G30" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K30" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="E31" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G31" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K31" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>48</v>
       </c>
+      <c r="C32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E32" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G32" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K32" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
       </c>
+      <c r="C33" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G33" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K33" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>48</v>
       </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G34" s="2" t="s">
         <v>71</v>
       </c>
       <c r="H34" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="E35" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G35" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K35" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
       </c>
+      <c r="C36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E36" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G36" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>48</v>
+      </c>
+      <c r="K36" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>48</v>
       </c>
+      <c r="C37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E37" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G37" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H37" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>48</v>
+      </c>
+      <c r="K37" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
+      <c r="E38" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H38" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>48</v>
+      </c>
+      <c r="K38" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="C39" t="s">
+        <v>48</v>
+      </c>
+      <c r="E39" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G39" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K39" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>48</v>
       </c>
+      <c r="C40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E40" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G40" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H40" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>48</v>
+      </c>
+      <c r="K40" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>48</v>
       </c>
+      <c r="C41" t="s">
+        <v>48</v>
+      </c>
+      <c r="E41" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G41" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K41" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>48</v>
       </c>
+      <c r="C42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E42" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G42" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K42" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
       </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G43" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K43" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="E44" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G44" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K44" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>48</v>
       </c>
+      <c r="C45" t="s">
+        <v>48</v>
+      </c>
+      <c r="E45" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G45" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K45" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>48</v>
       </c>
+      <c r="C46" t="s">
+        <v>48</v>
+      </c>
+      <c r="E46" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G46" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K46" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>48</v>
       </c>
+      <c r="C47" t="s">
+        <v>48</v>
+      </c>
+      <c r="E47" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
       <c r="G47" s="2" t="s">
         <v>78</v>
       </c>
       <c r="H47" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>48</v>
+      </c>
+      <c r="K47" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="E48" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G48" s="2" t="s">
         <v>79</v>
       </c>
       <c r="H48" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>48</v>
+      </c>
+      <c r="K48" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="E49" t="b">
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
       <c r="G49" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>48</v>
+      </c>
+      <c r="K49" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G50" s="2" t="s">
         <v>80</v>
       </c>
       <c r="H50" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>48</v>
+      </c>
+      <c r="K50" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G51" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K51" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G52" s="2" t="s">
         <v>82</v>
       </c>
       <c r="H52" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" t="s">
+        <v>48</v>
+      </c>
+      <c r="K52" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G53" s="2" t="s">
         <v>83</v>
       </c>
       <c r="H53" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>48</v>
+      </c>
+      <c r="K53" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G54" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H54" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>48</v>
+      </c>
+      <c r="K54" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G55" s="2" t="s">
         <v>84</v>
       </c>
       <c r="H55" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>48</v>
+      </c>
+      <c r="K55" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G56" s="2" t="s">
         <v>85</v>
       </c>
       <c r="H56" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K56" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G57" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K57" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G58" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H58" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K58" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G59" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H59" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>48</v>
+      </c>
+      <c r="K59" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G60" s="2" t="s">
         <v>27</v>
       </c>
       <c r="H60" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>48</v>
+      </c>
+      <c r="K60" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G61" s="2" t="s">
         <v>88</v>
       </c>
       <c r="H61" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>48</v>
+      </c>
+      <c r="K61" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G62" s="2" t="s">
         <v>89</v>
       </c>
       <c r="H62" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>48</v>
+      </c>
+      <c r="K62" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G63" s="2" t="s">
         <v>90</v>
       </c>
       <c r="H63" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>48</v>
+      </c>
+      <c r="K63" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G64" s="2" t="s">
         <v>28</v>
       </c>
       <c r="H64" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="65" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I64" t="s">
+        <v>48</v>
+      </c>
+      <c r="K64" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G65" s="2" t="s">
         <v>91</v>
       </c>
       <c r="H65" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="66" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>48</v>
+      </c>
+      <c r="K65" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G66" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="67" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K66" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G67" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="68" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K67" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G68" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="69" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K68" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G69" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="70" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K69" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H70" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="71" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K70" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G71" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H71" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="72" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>48</v>
+      </c>
+      <c r="K71" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G72" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="73" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K72" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G73" s="2" t="s">
         <v>32</v>
       </c>
       <c r="H73" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="74" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I73" t="s">
+        <v>48</v>
+      </c>
+      <c r="K73" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G74" s="2" t="s">
         <v>96</v>
       </c>
       <c r="H74" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="75" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I74" t="s">
+        <v>48</v>
+      </c>
+      <c r="K74" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G75" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="76" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K75" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G76" s="2" t="s">
         <v>34</v>
       </c>
       <c r="H76" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="77" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I76" t="s">
+        <v>48</v>
+      </c>
+      <c r="K76" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G77" s="2" t="s">
         <v>35</v>
       </c>
       <c r="H77" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="78" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I77" t="s">
+        <v>48</v>
+      </c>
+      <c r="K77" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G78" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="79" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I78" t="s">
+        <v>48</v>
+      </c>
+      <c r="K78" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G79" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="80" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K79" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G80" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="81" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K80" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G81" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="82" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K81" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G82" s="2" t="s">
         <v>38</v>
       </c>
       <c r="H82" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="83" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>48</v>
+      </c>
+      <c r="K82" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G83" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H83" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="84" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K83" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G84" s="2" t="s">
         <v>40</v>
       </c>
       <c r="H84" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="85" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I84" t="s">
+        <v>48</v>
+      </c>
+      <c r="K84" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G85" s="2" t="s">
         <v>41</v>
       </c>
       <c r="H85" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="86" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I85" t="s">
+        <v>48</v>
+      </c>
+      <c r="K85" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G86" s="2" t="s">
         <v>99</v>
       </c>
       <c r="H86" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="87" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
+        <v>48</v>
+      </c>
+      <c r="K86" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G87" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="88" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K87" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G88" s="2" t="s">
         <v>44</v>
       </c>
       <c r="H88" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="89" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I88" t="s">
+        <v>48</v>
+      </c>
+      <c r="K88" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G89" s="2" t="s">
         <v>45</v>
       </c>
       <c r="H89" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="90" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
+        <v>48</v>
+      </c>
+      <c r="K89" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G90" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="91" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K90" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G91" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="92" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="K91" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G92" s="2" t="s">
         <v>100</v>
       </c>
       <c r="H92" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="93" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="I92" t="s">
+        <v>48</v>
+      </c>
+      <c r="K92" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G93" s="2" t="s">
         <v>101</v>
+      </c>
+      <c r="K93" t="b">
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added yes/no for tag friendliness
</commit_message>
<xml_diff>
--- a/topic-files/Tag_Friendliness_8_Topics_and_16_Topics.xlsx
+++ b/topic-files/Tag_Friendliness_8_Topics_and_16_Topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creon/Desktop/UIUC/CS410/Team Project/CourseProject/topic-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SABreyals\CourseProject\topic-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7613FE00-5F6C-E649-B325-817718764F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEC178E-BDE9-4E12-8189-238A15850A86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="1460" windowWidth="33560" windowHeight="22640" xr2:uid="{C0B249B2-4F70-4EBF-AAE4-C111E07652C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C0B249B2-4F70-4EBF-AAE4-C111E07652C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="105">
   <si>
     <t>User-Friendly?</t>
   </si>
@@ -439,9 +439,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -466,6 +463,9 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -514,7 +514,7 @@
     <tableColumn id="2" xr3:uid="{D1A6DB4D-13DB-48D7-9E2B-C9FB047881F9}" name="Kurt"/>
     <tableColumn id="3" xr3:uid="{C7736CBA-5385-41C8-8441-2C8472818DBF}" name="Creon"/>
     <tableColumn id="4" xr3:uid="{BAFD5142-42F3-48E9-BF35-4EB4D5FD81CC}" name="Suhas"/>
-    <tableColumn id="5" xr3:uid="{113810B2-765C-F54B-A7C3-390459E3EE38}" name="Should Keep?" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{113810B2-765C-F54B-A7C3-390459E3EE38}" name="Should Keep?" dataDxfId="3">
       <calculatedColumnFormula>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -523,10 +523,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}" name="Table_16_Topics" displayName="Table_16_Topics" ref="G5:K93" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}" name="Table_16_Topics" displayName="Table_16_Topics" ref="G5:K93" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="G5:K93" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{891C3C5A-718E-41CB-BECD-51A095C7EA48}" name="Tag" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{891C3C5A-718E-41CB-BECD-51A095C7EA48}" name="Tag" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{342D09C5-EE2F-4797-AC7E-8C507A5D6470}" name="Kurt"/>
     <tableColumn id="3" xr3:uid="{1706DFBA-C6B1-4DC0-B09A-1674717EDFE0}" name="Creon"/>
     <tableColumn id="4" xr3:uid="{B49B5B10-9CB0-4EB0-AB00-0C83FC81E11F}" name="Suhas"/>
@@ -838,28 +838,28 @@
   <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="J92" sqref="J92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -877,7 +877,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -909,16 +909,19 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
       </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
       <c r="E6" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>52</v>
@@ -928,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -938,9 +941,12 @@
       <c r="C7" t="s">
         <v>48</v>
       </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
       <c r="E7" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>53</v>
@@ -950,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -960,9 +966,12 @@
       <c r="C8" t="s">
         <v>48</v>
       </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
       <c r="E8" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>4</v>
@@ -970,12 +979,15 @@
       <c r="I8" t="s">
         <v>48</v>
       </c>
+      <c r="J8" t="s">
+        <v>48</v>
+      </c>
       <c r="K8" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -985,19 +997,25 @@
       <c r="C9" t="s">
         <v>48</v>
       </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
       <c r="E9" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="J9" t="s">
+        <v>48</v>
+      </c>
       <c r="K9" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1007,9 +1025,12 @@
       <c r="C10" t="s">
         <v>48</v>
       </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
       <c r="E10" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>55</v>
@@ -1019,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1038,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1048,9 +1069,12 @@
       <c r="C12" t="s">
         <v>48</v>
       </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
       <c r="E12" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>57</v>
@@ -1066,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1083,12 +1107,15 @@
       <c r="I13" t="s">
         <v>48</v>
       </c>
+      <c r="J13" t="s">
+        <v>48</v>
+      </c>
       <c r="K13" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1105,12 +1132,15 @@
       <c r="I14" t="s">
         <v>48</v>
       </c>
+      <c r="J14" t="s">
+        <v>48</v>
+      </c>
       <c r="K14" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1120,9 +1150,12 @@
       <c r="C15" t="s">
         <v>48</v>
       </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
       <c r="E15" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>5</v>
@@ -1133,12 +1166,15 @@
       <c r="I15" t="s">
         <v>48</v>
       </c>
+      <c r="J15" t="s">
+        <v>48</v>
+      </c>
       <c r="K15" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1148,9 +1184,12 @@
       <c r="C16" t="s">
         <v>48</v>
       </c>
+      <c r="D16" t="s">
+        <v>48</v>
+      </c>
       <c r="E16" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>60</v>
@@ -1161,15 +1200,21 @@
       <c r="I16" t="s">
         <v>48</v>
       </c>
+      <c r="J16" t="s">
+        <v>48</v>
+      </c>
       <c r="K16" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
       <c r="E17" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
         <v>0</v>
@@ -1183,12 +1228,15 @@
       <c r="I17" t="s">
         <v>48</v>
       </c>
+      <c r="J17" t="s">
+        <v>48</v>
+      </c>
       <c r="K17" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1211,12 +1259,15 @@
       <c r="I18" t="s">
         <v>48</v>
       </c>
+      <c r="J18" t="s">
+        <v>48</v>
+      </c>
       <c r="K18" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1233,12 +1284,15 @@
       <c r="I19" t="s">
         <v>48</v>
       </c>
+      <c r="J19" t="s">
+        <v>48</v>
+      </c>
       <c r="K19" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1255,12 +1309,15 @@
       <c r="I20" t="s">
         <v>48</v>
       </c>
+      <c r="J20" t="s">
+        <v>48</v>
+      </c>
       <c r="K20" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1277,15 +1334,21 @@
       <c r="I21" t="s">
         <v>48</v>
       </c>
+      <c r="J21" t="s">
+        <v>48</v>
+      </c>
       <c r="K21" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
       <c r="E22" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
         <v>0</v>
@@ -1299,12 +1362,15 @@
       <c r="I22" t="s">
         <v>48</v>
       </c>
+      <c r="J22" t="s">
+        <v>48</v>
+      </c>
       <c r="K22" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1314,9 +1380,12 @@
       <c r="C23" t="s">
         <v>48</v>
       </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
       <c r="E23" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
@@ -1326,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1343,12 +1412,15 @@
       <c r="I24" t="s">
         <v>48</v>
       </c>
+      <c r="J24" t="s">
+        <v>48</v>
+      </c>
       <c r="K24" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1358,9 +1430,12 @@
       <c r="C25" t="s">
         <v>48</v>
       </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
       <c r="E25" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>65</v>
@@ -1370,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1380,9 +1455,12 @@
       <c r="C26" t="s">
         <v>48</v>
       </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
       <c r="E26" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>66</v>
@@ -1392,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1415,12 +1493,15 @@
       <c r="I27" t="s">
         <v>48</v>
       </c>
+      <c r="J27" t="s">
+        <v>48</v>
+      </c>
       <c r="K27" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1436,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1446,9 +1527,12 @@
       <c r="C29" t="s">
         <v>48</v>
       </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
       <c r="E29" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>67</v>
@@ -1461,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1471,9 +1555,12 @@
       <c r="C30" t="s">
         <v>48</v>
       </c>
+      <c r="D30" t="s">
+        <v>48</v>
+      </c>
       <c r="E30" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>68</v>
@@ -1483,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1499,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1509,9 +1596,12 @@
       <c r="C32" t="s">
         <v>48</v>
       </c>
+      <c r="D32" t="s">
+        <v>48</v>
+      </c>
       <c r="E32" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>12</v>
@@ -1521,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -1531,19 +1621,25 @@
       <c r="C33" t="s">
         <v>48</v>
       </c>
+      <c r="D33" t="s">
+        <v>48</v>
+      </c>
       <c r="E33" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="J33" t="s">
+        <v>48</v>
+      </c>
       <c r="K33" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -1553,9 +1649,12 @@
       <c r="C34" t="s">
         <v>48</v>
       </c>
+      <c r="D34" t="s">
+        <v>48</v>
+      </c>
       <c r="E34" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>71</v>
@@ -1566,12 +1665,15 @@
       <c r="I34" t="s">
         <v>48</v>
       </c>
+      <c r="J34" t="s">
+        <v>48</v>
+      </c>
       <c r="K34" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1582,12 +1684,15 @@
       <c r="G35" s="2" t="s">
         <v>72</v>
       </c>
+      <c r="J35" t="s">
+        <v>48</v>
+      </c>
       <c r="K35" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1597,9 +1702,12 @@
       <c r="C36" t="s">
         <v>48</v>
       </c>
+      <c r="D36" t="s">
+        <v>48</v>
+      </c>
       <c r="E36" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>73</v>
@@ -1607,12 +1715,15 @@
       <c r="I36" t="s">
         <v>48</v>
       </c>
+      <c r="J36" t="s">
+        <v>48</v>
+      </c>
       <c r="K36" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -1635,12 +1746,15 @@
       <c r="I37" t="s">
         <v>48</v>
       </c>
+      <c r="J37" t="s">
+        <v>48</v>
+      </c>
       <c r="K37" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -1657,21 +1771,27 @@
       <c r="I38" t="s">
         <v>48</v>
       </c>
+      <c r="J38" t="s">
+        <v>48</v>
+      </c>
       <c r="K38" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C39" t="s">
         <v>48</v>
       </c>
+      <c r="D39" t="s">
+        <v>48</v>
+      </c>
       <c r="E39" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>74</v>
@@ -1681,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -1691,9 +1811,12 @@
       <c r="C40" t="s">
         <v>48</v>
       </c>
+      <c r="D40" t="s">
+        <v>48</v>
+      </c>
       <c r="E40" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>16</v>
@@ -1709,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -1719,9 +1842,12 @@
       <c r="C41" t="s">
         <v>48</v>
       </c>
+      <c r="D41" t="s">
+        <v>48</v>
+      </c>
       <c r="E41" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>17</v>
@@ -1731,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -1741,9 +1867,12 @@
       <c r="C42" t="s">
         <v>48</v>
       </c>
+      <c r="D42" t="s">
+        <v>48</v>
+      </c>
       <c r="E42" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>75</v>
@@ -1753,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -1763,9 +1892,12 @@
       <c r="C43" t="s">
         <v>48</v>
       </c>
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
       <c r="E43" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>76</v>
@@ -1775,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -1791,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -1813,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -1823,19 +1955,25 @@
       <c r="C46" t="s">
         <v>48</v>
       </c>
+      <c r="D46" t="s">
+        <v>48</v>
+      </c>
       <c r="E46" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="J46" t="s">
+        <v>48</v>
+      </c>
       <c r="K46" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -1845,9 +1983,12 @@
       <c r="C47" t="s">
         <v>48</v>
       </c>
+      <c r="D47" t="s">
+        <v>48</v>
+      </c>
       <c r="E47" t="b">
         <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>78</v>
@@ -1863,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -1880,12 +2021,15 @@
       <c r="I48" t="s">
         <v>48</v>
       </c>
+      <c r="J48" t="s">
+        <v>48</v>
+      </c>
       <c r="K48" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -1902,12 +2046,15 @@
       <c r="I49" t="s">
         <v>48</v>
       </c>
+      <c r="J49" t="s">
+        <v>48</v>
+      </c>
       <c r="K49" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G50" s="2" t="s">
         <v>80</v>
       </c>
@@ -1922,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G51" s="2" t="s">
         <v>81</v>
       </c>
@@ -1931,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G52" s="2" t="s">
         <v>82</v>
       </c>
@@ -1941,12 +2088,15 @@
       <c r="I52" t="s">
         <v>48</v>
       </c>
+      <c r="J52" t="s">
+        <v>48</v>
+      </c>
       <c r="K52" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G53" s="2" t="s">
         <v>83</v>
       </c>
@@ -1956,12 +2106,15 @@
       <c r="I53" t="s">
         <v>48</v>
       </c>
+      <c r="J53" t="s">
+        <v>48</v>
+      </c>
       <c r="K53" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G54" s="2" t="s">
         <v>23</v>
       </c>
@@ -1971,12 +2124,15 @@
       <c r="I54" t="s">
         <v>48</v>
       </c>
+      <c r="J54" t="s">
+        <v>48</v>
+      </c>
       <c r="K54" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G55" s="2" t="s">
         <v>84</v>
       </c>
@@ -1986,12 +2142,15 @@
       <c r="I55" t="s">
         <v>48</v>
       </c>
+      <c r="J55" t="s">
+        <v>48</v>
+      </c>
       <c r="K55" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G56" s="2" t="s">
         <v>85</v>
       </c>
@@ -2003,28 +2162,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G57" s="2" t="s">
         <v>86</v>
       </c>
+      <c r="J57" t="s">
+        <v>48</v>
+      </c>
       <c r="K57" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G58" s="2" t="s">
         <v>87</v>
       </c>
       <c r="H58" t="s">
         <v>48</v>
       </c>
+      <c r="J58" t="s">
+        <v>48</v>
+      </c>
       <c r="K58" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G59" s="2" t="s">
         <v>24</v>
       </c>
@@ -2034,12 +2199,15 @@
       <c r="I59" t="s">
         <v>48</v>
       </c>
+      <c r="J59" t="s">
+        <v>48</v>
+      </c>
       <c r="K59" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G60" s="2" t="s">
         <v>27</v>
       </c>
@@ -2049,12 +2217,15 @@
       <c r="I60" t="s">
         <v>48</v>
       </c>
+      <c r="J60" t="s">
+        <v>48</v>
+      </c>
       <c r="K60" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G61" s="2" t="s">
         <v>88</v>
       </c>
@@ -2064,12 +2235,15 @@
       <c r="I61" t="s">
         <v>48</v>
       </c>
+      <c r="J61" t="s">
+        <v>48</v>
+      </c>
       <c r="K61" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G62" s="2" t="s">
         <v>89</v>
       </c>
@@ -2079,12 +2253,15 @@
       <c r="I62" t="s">
         <v>48</v>
       </c>
+      <c r="J62" t="s">
+        <v>48</v>
+      </c>
       <c r="K62" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G63" s="2" t="s">
         <v>90</v>
       </c>
@@ -2094,12 +2271,15 @@
       <c r="I63" t="s">
         <v>48</v>
       </c>
+      <c r="J63" t="s">
+        <v>48</v>
+      </c>
       <c r="K63" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G64" s="2" t="s">
         <v>28</v>
       </c>
@@ -2109,12 +2289,15 @@
       <c r="I64" t="s">
         <v>48</v>
       </c>
+      <c r="J64" t="s">
+        <v>48</v>
+      </c>
       <c r="K64" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G65" s="2" t="s">
         <v>91</v>
       </c>
@@ -2124,12 +2307,15 @@
       <c r="I65" t="s">
         <v>48</v>
       </c>
+      <c r="J65" t="s">
+        <v>48</v>
+      </c>
       <c r="K65" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G66" s="2" t="s">
         <v>92</v>
       </c>
@@ -2138,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G67" s="2" t="s">
         <v>93</v>
       </c>
@@ -2147,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G68" s="2" t="s">
         <v>94</v>
       </c>
@@ -2156,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G69" s="2" t="s">
         <v>29</v>
       </c>
@@ -2165,19 +2351,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G70" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H70" t="s">
         <v>48</v>
       </c>
+      <c r="J70" t="s">
+        <v>48</v>
+      </c>
       <c r="K70" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="7:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G71" s="2" t="s">
         <v>31</v>
       </c>
@@ -2187,12 +2376,15 @@
       <c r="I71" t="s">
         <v>48</v>
       </c>
+      <c r="J71" t="s">
+        <v>48</v>
+      </c>
       <c r="K71" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G72" s="2" t="s">
         <v>95</v>
       </c>
@@ -2201,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G73" s="2" t="s">
         <v>32</v>
       </c>
@@ -2211,12 +2403,15 @@
       <c r="I73" t="s">
         <v>48</v>
       </c>
+      <c r="J73" t="s">
+        <v>48</v>
+      </c>
       <c r="K73" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G74" s="2" t="s">
         <v>96</v>
       </c>
@@ -2226,12 +2421,15 @@
       <c r="I74" t="s">
         <v>48</v>
       </c>
+      <c r="J74" t="s">
+        <v>48</v>
+      </c>
       <c r="K74" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G75" s="2" t="s">
         <v>33</v>
       </c>
@@ -2240,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G76" s="2" t="s">
         <v>34</v>
       </c>
@@ -2250,12 +2448,15 @@
       <c r="I76" t="s">
         <v>48</v>
       </c>
+      <c r="J76" t="s">
+        <v>48</v>
+      </c>
       <c r="K76" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G77" s="2" t="s">
         <v>35</v>
       </c>
@@ -2270,19 +2471,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G78" s="2" t="s">
         <v>97</v>
       </c>
       <c r="I78" t="s">
         <v>48</v>
       </c>
+      <c r="J78" t="s">
+        <v>48</v>
+      </c>
       <c r="K78" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="7:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G79" s="2" t="s">
         <v>36</v>
       </c>
@@ -2291,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G80" s="2" t="s">
         <v>98</v>
       </c>
@@ -2300,16 +2504,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G81" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="J81" t="s">
+        <v>48</v>
+      </c>
       <c r="K81" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G82" s="2" t="s">
         <v>38</v>
       </c>
@@ -2319,24 +2526,30 @@
       <c r="I82" t="s">
         <v>48</v>
       </c>
+      <c r="J82" t="s">
+        <v>48</v>
+      </c>
       <c r="K82" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G83" s="2" t="s">
         <v>39</v>
       </c>
       <c r="H83" t="s">
         <v>48</v>
       </c>
+      <c r="J83" t="s">
+        <v>48</v>
+      </c>
       <c r="K83" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="7:11" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G84" s="2" t="s">
         <v>40</v>
       </c>
@@ -2346,12 +2559,15 @@
       <c r="I84" t="s">
         <v>48</v>
       </c>
+      <c r="J84" t="s">
+        <v>48</v>
+      </c>
       <c r="K84" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G85" s="2" t="s">
         <v>41</v>
       </c>
@@ -2361,12 +2577,15 @@
       <c r="I85" t="s">
         <v>48</v>
       </c>
+      <c r="J85" t="s">
+        <v>48</v>
+      </c>
       <c r="K85" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G86" s="2" t="s">
         <v>99</v>
       </c>
@@ -2376,12 +2595,15 @@
       <c r="I86" t="s">
         <v>48</v>
       </c>
+      <c r="J86" t="s">
+        <v>48</v>
+      </c>
       <c r="K86" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G87" s="2" t="s">
         <v>42</v>
       </c>
@@ -2390,7 +2612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G88" s="2" t="s">
         <v>44</v>
       </c>
@@ -2400,12 +2622,15 @@
       <c r="I88" t="s">
         <v>48</v>
       </c>
+      <c r="J88" t="s">
+        <v>48</v>
+      </c>
       <c r="K88" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G89" s="2" t="s">
         <v>45</v>
       </c>
@@ -2415,12 +2640,15 @@
       <c r="I89" t="s">
         <v>48</v>
       </c>
+      <c r="J89" t="s">
+        <v>48</v>
+      </c>
       <c r="K89" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G90" s="2" t="s">
         <v>46</v>
       </c>
@@ -2429,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G91" s="2" t="s">
         <v>47</v>
       </c>
@@ -2438,7 +2666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="7:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G92" s="2" t="s">
         <v>100</v>
       </c>
@@ -2448,12 +2676,15 @@
       <c r="I92" t="s">
         <v>48</v>
       </c>
+      <c r="J92" t="s">
+        <v>48</v>
+      </c>
       <c r="K92" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="7:11" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G93" s="2" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
Tweaked Tag_Friendliness_8_Topics_and_16_Topics.xlsx to mark tags to keep if at least 2/3 of project members vote to keep.
</commit_message>
<xml_diff>
--- a/topic-files/Tag_Friendliness_8_Topics_and_16_Topics.xlsx
+++ b/topic-files/Tag_Friendliness_8_Topics_and_16_Topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SABreyals\CourseProject\topic-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_410_Text_Info_Systems\Project\CourseProject\topic-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEC178E-BDE9-4E12-8189-238A15850A86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9762A2-29D2-4119-9010-DDAF9E4E6574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C0B249B2-4F70-4EBF-AAE4-C111E07652C1}"/>
+    <workbookView xWindow="31550" yWindow="950" windowWidth="18690" windowHeight="18410" xr2:uid="{C0B249B2-4F70-4EBF-AAE4-C111E07652C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,6 +439,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -463,9 +466,6 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -514,8 +514,8 @@
     <tableColumn id="2" xr3:uid="{D1A6DB4D-13DB-48D7-9E2B-C9FB047881F9}" name="Kurt"/>
     <tableColumn id="3" xr3:uid="{C7736CBA-5385-41C8-8441-2C8472818DBF}" name="Creon"/>
     <tableColumn id="4" xr3:uid="{BAFD5142-42F3-48E9-BF35-4EB4D5FD81CC}" name="Suhas"/>
-    <tableColumn id="5" xr3:uid="{113810B2-765C-F54B-A7C3-390459E3EE38}" name="Should Keep?" dataDxfId="3">
-      <calculatedColumnFormula>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{113810B2-765C-F54B-A7C3-390459E3EE38}" name="Should Keep?" dataDxfId="1">
+      <calculatedColumnFormula>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -523,15 +523,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}" name="Table_16_Topics" displayName="Table_16_Topics" ref="G5:K93" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}" name="Table_16_Topics" displayName="Table_16_Topics" ref="G5:K93" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="G5:K93" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{891C3C5A-718E-41CB-BECD-51A095C7EA48}" name="Tag" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{891C3C5A-718E-41CB-BECD-51A095C7EA48}" name="Tag" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{342D09C5-EE2F-4797-AC7E-8C507A5D6470}" name="Kurt"/>
     <tableColumn id="3" xr3:uid="{1706DFBA-C6B1-4DC0-B09A-1674717EDFE0}" name="Creon"/>
     <tableColumn id="4" xr3:uid="{B49B5B10-9CB0-4EB0-AB00-0C83FC81E11F}" name="Suhas"/>
     <tableColumn id="5" xr3:uid="{CBEE1EE4-5DE5-6942-AC94-BA3C3CDC6AA5}" name="Should Keep?" dataDxfId="0">
-      <calculatedColumnFormula>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</calculatedColumnFormula>
+      <calculatedColumnFormula>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -838,7 +838,7 @@
   <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J92" sqref="J92"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,14 +920,14 @@
         <v>48</v>
       </c>
       <c r="E6" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="K6" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -945,14 +945,14 @@
         <v>48</v>
       </c>
       <c r="E7" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="K7" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -970,8 +970,8 @@
         <v>48</v>
       </c>
       <c r="E8" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>4</v>
@@ -983,7 +983,7 @@
         <v>48</v>
       </c>
       <c r="K8" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -1001,8 +1001,8 @@
         <v>48</v>
       </c>
       <c r="E9" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>54</v>
@@ -1011,7 +1011,7 @@
         <v>48</v>
       </c>
       <c r="K9" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1029,14 +1029,14 @@
         <v>48</v>
       </c>
       <c r="E10" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>55</v>
       </c>
       <c r="K10" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1045,7 +1045,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
@@ -1055,7 +1055,7 @@
         <v>48</v>
       </c>
       <c r="K11" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1073,8 +1073,8 @@
         <v>48</v>
       </c>
       <c r="E12" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>57</v>
@@ -1086,7 +1086,7 @@
         <v>48</v>
       </c>
       <c r="K12" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -1095,7 +1095,7 @@
         <v>11</v>
       </c>
       <c r="E13" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -1111,8 +1111,8 @@
         <v>48</v>
       </c>
       <c r="K13" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
         <v>12</v>
       </c>
       <c r="E14" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -1136,8 +1136,8 @@
         <v>48</v>
       </c>
       <c r="K14" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1154,8 +1154,8 @@
         <v>48</v>
       </c>
       <c r="E15" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>5</v>
@@ -1170,8 +1170,8 @@
         <v>48</v>
       </c>
       <c r="K15" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1188,8 +1188,8 @@
         <v>48</v>
       </c>
       <c r="E16" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>60</v>
@@ -1204,8 +1204,8 @@
         <v>48</v>
       </c>
       <c r="K16" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1216,7 +1216,7 @@
         <v>48</v>
       </c>
       <c r="E17" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -1232,8 +1232,8 @@
         <v>48</v>
       </c>
       <c r="K17" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>48</v>
       </c>
       <c r="E18" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
@@ -1263,8 +1263,8 @@
         <v>48</v>
       </c>
       <c r="K18" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1272,7 +1272,7 @@
         <v>17</v>
       </c>
       <c r="E19" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G19" s="2" t="s">
@@ -1288,8 +1288,8 @@
         <v>48</v>
       </c>
       <c r="K19" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1297,7 +1297,7 @@
         <v>18</v>
       </c>
       <c r="E20" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G20" s="2" t="s">
@@ -1313,8 +1313,8 @@
         <v>48</v>
       </c>
       <c r="K20" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1322,7 +1322,7 @@
         <v>19</v>
       </c>
       <c r="E21" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -1338,8 +1338,8 @@
         <v>48</v>
       </c>
       <c r="K21" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1350,7 +1350,7 @@
         <v>48</v>
       </c>
       <c r="E22" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -1366,8 +1366,8 @@
         <v>48</v>
       </c>
       <c r="K22" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1384,14 +1384,14 @@
         <v>48</v>
       </c>
       <c r="E23" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K23" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
         <v>22</v>
       </c>
       <c r="E24" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -1416,8 +1416,8 @@
         <v>48</v>
       </c>
       <c r="K24" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1434,14 +1434,14 @@
         <v>48</v>
       </c>
       <c r="E25" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>65</v>
       </c>
       <c r="K25" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1459,14 +1459,14 @@
         <v>48</v>
       </c>
       <c r="E26" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>66</v>
       </c>
       <c r="K26" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
         <v>48</v>
       </c>
       <c r="E27" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
@@ -1497,8 +1497,8 @@
         <v>48</v>
       </c>
       <c r="K27" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1506,14 +1506,14 @@
         <v>26</v>
       </c>
       <c r="E28" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>11</v>
       </c>
       <c r="K28" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1531,8 +1531,8 @@
         <v>48</v>
       </c>
       <c r="E29" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>67</v>
@@ -1541,7 +1541,7 @@
         <v>48</v>
       </c>
       <c r="K29" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1559,14 +1559,14 @@
         <v>48</v>
       </c>
       <c r="E30" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>68</v>
       </c>
       <c r="K30" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1575,14 +1575,14 @@
         <v>29</v>
       </c>
       <c r="E31" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>69</v>
       </c>
       <c r="K31" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1600,14 +1600,14 @@
         <v>48</v>
       </c>
       <c r="E32" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K32" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1625,8 +1625,8 @@
         <v>48</v>
       </c>
       <c r="E33" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>70</v>
@@ -1635,7 +1635,7 @@
         <v>48</v>
       </c>
       <c r="K33" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1653,8 +1653,8 @@
         <v>48</v>
       </c>
       <c r="E34" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>71</v>
@@ -1669,8 +1669,8 @@
         <v>48</v>
       </c>
       <c r="K34" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -1678,7 +1678,7 @@
         <v>33</v>
       </c>
       <c r="E35" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G35" s="2" t="s">
@@ -1688,7 +1688,7 @@
         <v>48</v>
       </c>
       <c r="K35" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1706,8 +1706,8 @@
         <v>48</v>
       </c>
       <c r="E36" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>73</v>
@@ -1719,7 +1719,7 @@
         <v>48</v>
       </c>
       <c r="K36" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
         <v>48</v>
       </c>
       <c r="E37" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
@@ -1750,8 +1750,8 @@
         <v>48</v>
       </c>
       <c r="K37" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>36</v>
       </c>
       <c r="E38" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G38" s="2" t="s">
@@ -1775,8 +1775,8 @@
         <v>48</v>
       </c>
       <c r="K38" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -1790,14 +1790,14 @@
         <v>48</v>
       </c>
       <c r="E39" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>74</v>
       </c>
       <c r="K39" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1815,8 +1815,8 @@
         <v>48</v>
       </c>
       <c r="E40" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>16</v>
@@ -1828,7 +1828,7 @@
         <v>48</v>
       </c>
       <c r="K40" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -1846,14 +1846,14 @@
         <v>48</v>
       </c>
       <c r="E41" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>17</v>
       </c>
       <c r="K41" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1871,14 +1871,14 @@
         <v>48</v>
       </c>
       <c r="E42" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>75</v>
       </c>
       <c r="K42" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1896,14 +1896,14 @@
         <v>48</v>
       </c>
       <c r="E43" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>76</v>
       </c>
       <c r="K43" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1912,14 +1912,14 @@
         <v>42</v>
       </c>
       <c r="E44" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>77</v>
       </c>
       <c r="K44" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1934,14 +1934,14 @@
         <v>48</v>
       </c>
       <c r="E45" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>19</v>
       </c>
       <c r="K45" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1959,8 +1959,8 @@
         <v>48</v>
       </c>
       <c r="E46" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>20</v>
@@ -1969,7 +1969,7 @@
         <v>48</v>
       </c>
       <c r="K46" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -1987,8 +1987,8 @@
         <v>48</v>
       </c>
       <c r="E47" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>78</v>
@@ -2000,7 +2000,7 @@
         <v>48</v>
       </c>
       <c r="K47" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -2009,7 +2009,7 @@
         <v>46</v>
       </c>
       <c r="E48" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G48" s="2" t="s">
@@ -2025,8 +2025,8 @@
         <v>48</v>
       </c>
       <c r="K48" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -2034,7 +2034,7 @@
         <v>47</v>
       </c>
       <c r="E49" t="b">
-        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
       <c r="G49" s="2" t="s">
@@ -2050,8 +2050,8 @@
         <v>48</v>
       </c>
       <c r="K49" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2065,7 +2065,7 @@
         <v>48</v>
       </c>
       <c r="K50" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -2074,7 +2074,7 @@
         <v>81</v>
       </c>
       <c r="K51" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2092,8 +2092,8 @@
         <v>48</v>
       </c>
       <c r="K52" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -2110,8 +2110,8 @@
         <v>48</v>
       </c>
       <c r="K53" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -2128,8 +2128,8 @@
         <v>48</v>
       </c>
       <c r="K54" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -2146,8 +2146,8 @@
         <v>48</v>
       </c>
       <c r="K55" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>48</v>
       </c>
       <c r="K56" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2170,7 +2170,7 @@
         <v>48</v>
       </c>
       <c r="K57" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2185,7 +2185,7 @@
         <v>48</v>
       </c>
       <c r="K58" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -2203,8 +2203,8 @@
         <v>48</v>
       </c>
       <c r="K59" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2221,8 +2221,8 @@
         <v>48</v>
       </c>
       <c r="K60" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2239,8 +2239,8 @@
         <v>48</v>
       </c>
       <c r="K61" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -2257,8 +2257,8 @@
         <v>48</v>
       </c>
       <c r="K62" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2275,8 +2275,8 @@
         <v>48</v>
       </c>
       <c r="K63" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -2293,8 +2293,8 @@
         <v>48</v>
       </c>
       <c r="K64" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="7:11" x14ac:dyDescent="0.25">
@@ -2311,8 +2311,8 @@
         <v>48</v>
       </c>
       <c r="K65" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="7:11" x14ac:dyDescent="0.25">
@@ -2320,7 +2320,7 @@
         <v>92</v>
       </c>
       <c r="K66" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2329,7 +2329,7 @@
         <v>93</v>
       </c>
       <c r="K67" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2338,7 +2338,7 @@
         <v>94</v>
       </c>
       <c r="K68" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2347,7 +2347,7 @@
         <v>29</v>
       </c>
       <c r="K69" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2362,7 +2362,7 @@
         <v>48</v>
       </c>
       <c r="K70" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -2380,8 +2380,8 @@
         <v>48</v>
       </c>
       <c r="K71" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="7:11" x14ac:dyDescent="0.25">
@@ -2389,7 +2389,7 @@
         <v>95</v>
       </c>
       <c r="K72" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2407,8 +2407,8 @@
         <v>48</v>
       </c>
       <c r="K73" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="7:11" x14ac:dyDescent="0.25">
@@ -2425,8 +2425,8 @@
         <v>48</v>
       </c>
       <c r="K74" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="7:11" x14ac:dyDescent="0.25">
@@ -2434,7 +2434,7 @@
         <v>33</v>
       </c>
       <c r="K75" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2452,8 +2452,8 @@
         <v>48</v>
       </c>
       <c r="K76" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="7:11" x14ac:dyDescent="0.25">
@@ -2467,7 +2467,7 @@
         <v>48</v>
       </c>
       <c r="K77" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -2482,7 +2482,7 @@
         <v>48</v>
       </c>
       <c r="K78" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -2491,7 +2491,7 @@
         <v>36</v>
       </c>
       <c r="K79" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2500,7 +2500,7 @@
         <v>98</v>
       </c>
       <c r="K80" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
         <v>48</v>
       </c>
       <c r="K81" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2530,8 +2530,8 @@
         <v>48</v>
       </c>
       <c r="K82" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="7:11" x14ac:dyDescent="0.25">
@@ -2545,7 +2545,7 @@
         <v>48</v>
       </c>
       <c r="K83" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>1</v>
       </c>
     </row>
@@ -2563,8 +2563,8 @@
         <v>48</v>
       </c>
       <c r="K84" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="7:11" x14ac:dyDescent="0.25">
@@ -2581,8 +2581,8 @@
         <v>48</v>
       </c>
       <c r="K85" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="7:11" x14ac:dyDescent="0.25">
@@ -2599,8 +2599,8 @@
         <v>48</v>
       </c>
       <c r="K86" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="7:11" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
         <v>42</v>
       </c>
       <c r="K87" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2626,8 +2626,8 @@
         <v>48</v>
       </c>
       <c r="K88" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="7:11" x14ac:dyDescent="0.25">
@@ -2644,8 +2644,8 @@
         <v>48</v>
       </c>
       <c r="K89" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="7:11" x14ac:dyDescent="0.25">
@@ -2653,7 +2653,7 @@
         <v>46</v>
       </c>
       <c r="K90" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2662,7 +2662,7 @@
         <v>47</v>
       </c>
       <c r="K91" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>
@@ -2680,8 +2680,8 @@
         <v>48</v>
       </c>
       <c r="K92" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
-        <v>0</v>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="7:11" x14ac:dyDescent="0.25">
@@ -2689,7 +2689,7 @@
         <v>101</v>
       </c>
       <c r="K93" t="b">
-        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")=2</f>
+        <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed underscores from tags. Deleted 8 and 16 versions of output
</commit_message>
<xml_diff>
--- a/topic-files/Tag_Friendliness_8_Topics_and_16_Topics.xlsx
+++ b/topic-files/Tag_Friendliness_8_Topics_and_16_Topics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktuoh\Documents\School\MCS-DS\CS_410_Text_Info_Systems\Project\CourseProject\topic-files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/creon/Desktop/UIUC/CS410/Team Project/CourseProject/topic-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9762A2-29D2-4119-9010-DDAF9E4E6574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6F7B3D-3BBE-294A-90FC-023CFFAA0BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31550" yWindow="950" windowWidth="18690" windowHeight="18410" xr2:uid="{C0B249B2-4F70-4EBF-AAE4-C111E07652C1}"/>
+    <workbookView xWindow="13560" yWindow="960" windowWidth="36700" windowHeight="22120" xr2:uid="{C0B249B2-4F70-4EBF-AAE4-C111E07652C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="105">
   <si>
     <t>User-Friendly?</t>
   </si>
@@ -439,9 +439,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -466,6 +463,9 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -514,7 +514,7 @@
     <tableColumn id="2" xr3:uid="{D1A6DB4D-13DB-48D7-9E2B-C9FB047881F9}" name="Kurt"/>
     <tableColumn id="3" xr3:uid="{C7736CBA-5385-41C8-8441-2C8472818DBF}" name="Creon"/>
     <tableColumn id="4" xr3:uid="{BAFD5142-42F3-48E9-BF35-4EB4D5FD81CC}" name="Suhas"/>
-    <tableColumn id="5" xr3:uid="{113810B2-765C-F54B-A7C3-390459E3EE38}" name="Should Keep?" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{113810B2-765C-F54B-A7C3-390459E3EE38}" name="Should Keep?" dataDxfId="3">
       <calculatedColumnFormula>COUNTIF(Table_8_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -523,10 +523,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}" name="Table_16_Topics" displayName="Table_16_Topics" ref="G5:K93" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}" name="Table_16_Topics" displayName="Table_16_Topics" ref="G5:K93" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="G5:K93" xr:uid="{D0CD3E9E-424D-4CF8-996A-DC1F6BBA5F37}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{891C3C5A-718E-41CB-BECD-51A095C7EA48}" name="Tag" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{891C3C5A-718E-41CB-BECD-51A095C7EA48}" name="Tag" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{342D09C5-EE2F-4797-AC7E-8C507A5D6470}" name="Kurt"/>
     <tableColumn id="3" xr3:uid="{1706DFBA-C6B1-4DC0-B09A-1674717EDFE0}" name="Creon"/>
     <tableColumn id="4" xr3:uid="{B49B5B10-9CB0-4EB0-AB00-0C83FC81E11F}" name="Suhas"/>
@@ -838,28 +838,28 @@
   <dimension ref="A1:K93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="L81" sqref="L81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="11" max="11" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>49</v>
       </c>
@@ -877,7 +877,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -909,7 +909,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -931,7 +931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -987,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1236,7 +1236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -1857,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -1973,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G50" s="2" t="s">
         <v>80</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G51" s="2" t="s">
         <v>81</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G52" s="2" t="s">
         <v>82</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G53" s="2" t="s">
         <v>83</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G54" s="2" t="s">
         <v>23</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G55" s="2" t="s">
         <v>84</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G56" s="2" t="s">
         <v>85</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G57" s="2" t="s">
         <v>86</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G58" s="2" t="s">
         <v>87</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G59" s="2" t="s">
         <v>24</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G60" s="2" t="s">
         <v>27</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G61" s="2" t="s">
         <v>88</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G62" s="2" t="s">
         <v>89</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G63" s="2" t="s">
         <v>90</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="G64" s="2" t="s">
         <v>28</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G65" s="2" t="s">
         <v>91</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G66" s="2" t="s">
         <v>92</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G67" s="2" t="s">
         <v>93</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G68" s="2" t="s">
         <v>94</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G69" s="2" t="s">
         <v>29</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G70" s="2" t="s">
         <v>30</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G71" s="2" t="s">
         <v>31</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G72" s="2" t="s">
         <v>95</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G73" s="2" t="s">
         <v>32</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G74" s="2" t="s">
         <v>96</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G75" s="2" t="s">
         <v>33</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G76" s="2" t="s">
         <v>34</v>
       </c>
@@ -2456,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G77" s="2" t="s">
         <v>35</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G78" s="2" t="s">
         <v>97</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G79" s="2" t="s">
         <v>36</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G80" s="2" t="s">
         <v>98</v>
       </c>
@@ -2504,19 +2504,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G81" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="I81" t="s">
+        <v>48</v>
+      </c>
       <c r="J81" t="s">
         <v>48</v>
       </c>
       <c r="K81" t="b">
         <f>COUNTIF(Table_16_Topics[[#This Row],[Kurt]:[Suhas]],"yes")&gt;=2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="7:11" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G82" s="2" t="s">
         <v>38</v>
       </c>
@@ -2534,7 +2537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G83" s="2" t="s">
         <v>39</v>
       </c>
@@ -2549,7 +2552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G84" s="2" t="s">
         <v>40</v>
       </c>
@@ -2567,7 +2570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G85" s="2" t="s">
         <v>41</v>
       </c>
@@ -2585,7 +2588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G86" s="2" t="s">
         <v>99</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G87" s="2" t="s">
         <v>42</v>
       </c>
@@ -2612,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G88" s="2" t="s">
         <v>44</v>
       </c>
@@ -2630,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G89" s="2" t="s">
         <v>45</v>
       </c>
@@ -2648,7 +2651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G90" s="2" t="s">
         <v>46</v>
       </c>
@@ -2657,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G91" s="2" t="s">
         <v>47</v>
       </c>
@@ -2666,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G92" s="2" t="s">
         <v>100</v>
       </c>
@@ -2684,7 +2687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="7:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="7:11" x14ac:dyDescent="0.2">
       <c r="G93" s="2" t="s">
         <v>101</v>
       </c>

</xml_diff>